<commit_message>
add gff_path to diphtheriae metadata
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/Cdiphtheriae_test_metadata.xlsx
+++ b/assets/sample_metadata/Cdiphtheriae_test_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78F0DB9-D91D-4C1B-A1B8-ECFB378A45F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2C640A-7EBC-4B15-80A5-6C0E39743660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="2250" windowWidth="21600" windowHeight="11265" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
   <si>
     <t>Submission info</t>
   </si>
@@ -273,13 +273,22 @@
   </si>
   <si>
     <t>BX248355</t>
+  </si>
+  <si>
+    <t>gff_path</t>
+  </si>
+  <si>
+    <t>assets/sample_annotations/Cdiphtheriae/CP040557.gff</t>
+  </si>
+  <si>
+    <t>assets/sample_annotations/Cdiphtheriae/BX248355.gff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,8 +310,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +328,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF8FAADC"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8FAADC"/>
       </patternFill>
     </fill>
   </fills>
@@ -381,7 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -397,6 +417,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -714,18 +737,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
-  <dimension ref="A1:AZ4"/>
+  <dimension ref="A1:BA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AN4" sqref="AN4"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AL8" sqref="AL8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="47" width="24" customWidth="1"/>
+    <col min="1" max="48" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,13 +788,13 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
@@ -779,10 +802,10 @@
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
-      <c r="AP1" s="2" t="s">
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
@@ -792,8 +815,9 @@
       <c r="AX1" s="1"/>
       <c r="AY1" s="1"/>
       <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
     </row>
-    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -887,69 +911,72 @@
       <c r="AE2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AF2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AU2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="4" t="s">
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -1012,24 +1039,26 @@
         <v>71</v>
       </c>
       <c r="AF3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
-      <c r="AM3" s="1" t="s">
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN3" s="1" t="s">
+      <c r="AO3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AO3" s="1" t="s">
+      <c r="AP3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
       <c r="AS3" s="1"/>
@@ -1040,8 +1069,9 @@
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
       <c r="AZ3" s="1"/>
+      <c r="BA3" s="1"/>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>78</v>
       </c>
@@ -1104,24 +1134,26 @@
         <v>72</v>
       </c>
       <c r="AF4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG4" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
-      <c r="AM4" s="1" t="s">
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN4" s="1" t="s">
+      <c r="AO4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AO4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
       <c r="AS4" s="1"/>
@@ -1132,6 +1164,7 @@
       <c r="AX4" s="1"/>
       <c r="AY4" s="1"/>
       <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bacteria test file was missing a BioProject ID and gff_path column
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/Cdiphtheriae_test_metadata.xlsx
+++ b/assets/sample_metadata/Cdiphtheriae_test_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\sample_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FEFE96-46EB-4B24-A20B-DBE0C8A06C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76982FD9-E7B4-4810-8A78-02A0F949DC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="1990" yWindow="7980" windowWidth="19180" windowHeight="11380" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="88">
   <si>
     <t>Submission info</t>
   </si>
@@ -288,6 +288,18 @@
   </si>
   <si>
     <t>authors</t>
+  </si>
+  <si>
+    <t>PRJNA541849</t>
+  </si>
+  <si>
+    <t>gff_path</t>
+  </si>
+  <si>
+    <t>assets/sample_annotations/Cdiphtheriae/CP040557.gff</t>
+  </si>
+  <si>
+    <t>assets/sample_annotations/Cdiphtheriae/BX248355.gff</t>
   </si>
 </sst>
 </file>
@@ -749,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
-  <dimension ref="A1:BD45"/>
+  <dimension ref="A1:BE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -760,10 +772,10 @@
     <col min="1" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="24.1796875" customWidth="1"/>
     <col min="6" max="6" width="23.453125" customWidth="1"/>
-    <col min="7" max="51" width="24" customWidth="1"/>
+    <col min="7" max="52" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,13 +818,13 @@
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -820,10 +832,10 @@
       <c r="AQ1" s="1"/>
       <c r="AR1" s="1"/>
       <c r="AS1" s="1"/>
-      <c r="AT1" s="2" t="s">
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
       <c r="AW1" s="1"/>
       <c r="AX1" s="1"/>
@@ -833,8 +845,9 @@
       <c r="BB1" s="1"/>
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
-    </row>
-    <row r="2" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BE1" s="1"/>
+    </row>
+    <row r="2" spans="1:57" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -940,69 +953,72 @@
       <c r="AI2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AJ2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="BA2" s="1"/>
-      <c r="BB2" s="4" t="s">
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
@@ -1012,7 +1028,9 @@
       <c r="C3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="E3" t="s">
         <v>82</v>
       </c>
@@ -1073,24 +1091,26 @@
         <v>70</v>
       </c>
       <c r="AJ3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
-      <c r="AQ3" s="1" t="s">
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AS3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AT3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
@@ -1101,8 +1121,9 @@
       <c r="BB3" s="1"/>
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
-    </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="BE3" s="1"/>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>77</v>
       </c>
@@ -1112,7 +1133,9 @@
       <c r="C4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="E4" t="s">
         <v>82</v>
       </c>
@@ -1173,24 +1196,26 @@
         <v>71</v>
       </c>
       <c r="AJ4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
-      <c r="AQ4" s="1" t="s">
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AR4" s="1" t="s">
+      <c r="AS4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
@@ -1201,29 +1226,30 @@
       <c r="BB4" s="1"/>
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
-    </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.35">
+      <c r="BE4" s="1"/>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.35">
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
corrections to submission.xml files and changes to variable names for host_sex host_age geo_loc_name
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/Cdiphtheriae_test_metadata.xlsx
+++ b/assets/sample_metadata/Cdiphtheriae_test_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76982FD9-E7B4-4810-8A78-02A0F949DC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594FD5BB-1E30-4683-9BF5-6EB07A15CAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1990" yWindow="7980" windowWidth="19180" windowHeight="11380" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D029CB50-4CB9-4BD3-B61F-E5821D8D6205}"/>
   </bookViews>
   <sheets>
     <sheet name="Diphtheria_Metadata" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="87">
   <si>
     <t>Submission info</t>
   </si>
@@ -86,12 +86,6 @@
     <t>purpose_of_sampling</t>
   </si>
   <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
     <t>race</t>
   </si>
   <si>
@@ -266,9 +260,6 @@
     <t>assets/sample_fastqs/Cdiphtheriae/BX248355_R2.fastq.gz</t>
   </si>
   <si>
-    <t>BX248355.1</t>
-  </si>
-  <si>
     <t>BX248355</t>
   </si>
   <si>
@@ -296,10 +287,16 @@
     <t>gff_path</t>
   </si>
   <si>
-    <t>assets/sample_annotations/Cdiphtheriae/CP040557.gff</t>
-  </si>
-  <si>
-    <t>assets/sample_annotations/Cdiphtheriae/BX248355.gff</t>
+    <t>assets/sample_annotations/Cdiphtheriae/CP040557.gff3</t>
+  </si>
+  <si>
+    <t>assets/sample_annotations/Cdiphtheriae/BX248355.gff3</t>
+  </si>
+  <si>
+    <t>host_sex</t>
+  </si>
+  <si>
+    <t>host_age</t>
   </si>
 </sst>
 </file>
@@ -763,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43A21E4-DEDF-48C8-84DE-AC4607355643}">
   <dimension ref="A1:BE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -820,10 +817,10 @@
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
@@ -834,7 +831,7 @@
       <c r="AS1" s="1"/>
       <c r="AT1" s="1"/>
       <c r="AU1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AV1" s="1"/>
       <c r="AW1" s="1"/>
@@ -852,46 +849,46 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>6</v>
@@ -924,158 +921,158 @@
         <v>15</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AB2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AF2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AH2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AI2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AL2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="AI2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AJ2" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AM2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AN2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AS2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AQ2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AS2" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="AT2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AW2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="AZ2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="BA2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="BB2" s="1"/>
       <c r="BC2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BE2" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="BD2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="BE2" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
@@ -1088,13 +1085,13 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
@@ -1103,13 +1100,13 @@
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AS3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT3" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="AT3" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
@@ -1125,62 +1122,62 @@
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="U4" s="1"/>
       <c r="V4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
@@ -1193,13 +1190,13 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
@@ -1208,13 +1205,13 @@
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AS4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT4" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="AT4" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>

</xml_diff>